<commit_message>
push script and execute
</commit_message>
<xml_diff>
--- a/Input_data/Inputs.xlsx
+++ b/Input_data/Inputs.xlsx
@@ -4,24 +4,67 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815"/>
+    <workbookView windowWidth="19815" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Valid Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Verify Product Version " sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Title of home page</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>actiTIME - Enter Time-Track</t>
+  </si>
+  <si>
+    <t>ErrMsg</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Username or Password is invalid. Please try again.</t>
+  </si>
+  <si>
+    <t>admin1</t>
+  </si>
+  <si>
+    <t>Product Version</t>
+  </si>
+  <si>
+    <t>actiTIME 2020 Online</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -30,6 +73,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -39,14 +119,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -55,14 +128,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -76,6 +141,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -107,16 +180,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,29 +197,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,37 +233,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,7 +377,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,143 +413,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -388,15 +453,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -419,8 +475,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -436,6 +501,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -457,15 +531,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -479,7 +544,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -488,146 +559,142 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,14 +1014,157 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="3" max="3" width="27.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="16.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.2857142857143" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="2:3">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="9.14285714285714" style="1"/>
+    <col min="2" max="2" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7142857142857" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>